<commit_message>
Updated space_details related numbers
</commit_message>
<xml_diff>
--- a/python/BytheNumbersAdditionalData.xlsx
+++ b/python/BytheNumbersAdditionalData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TaoWork\webapps\Numbers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HeardGit\dashboard\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F6C6B-1C31-4B1B-A8E1-180E822A7D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BDD75E-3009-40BD-8B86-D71F7739DC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="830" windowWidth="16970" windowHeight="9370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8240" yWindow="0" windowWidth="10260" windowHeight="9370" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DigitalCollection" sheetId="2" r:id="rId1"/>
     <sheet name="SpaceDetails" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Included with ARL counts. 4948 available;  198 withheld; etd_available; etd_withheld (withheld items are not available to the public)</t>
   </si>
@@ -194,6 +195,54 @@
   </si>
   <si>
     <t>from Cliff</t>
+  </si>
+  <si>
+    <t># of personnel</t>
+  </si>
+  <si>
+    <t>Acquisitions &amp; E-Resources</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Annex</t>
+  </si>
+  <si>
+    <t>Assessment, Communication &amp; Engagement</t>
+  </si>
+  <si>
+    <t>Library Unit</t>
+  </si>
+  <si>
+    <t>Cataloging &amp; Metadata</t>
+  </si>
+  <si>
+    <t>Collections &amp; Collections Services</t>
+  </si>
+  <si>
+    <t>Core Services</t>
+  </si>
+  <si>
+    <t>Digital Scholarship &amp; Communications</t>
+  </si>
+  <si>
+    <t>History of Medicine Collections</t>
+  </si>
+  <si>
+    <t>Interlibrary Loan</t>
+  </si>
+  <si>
+    <t>Library Technology and Digital Services</t>
+  </si>
+  <si>
+    <t>Preservation</t>
+  </si>
+  <si>
+    <t>Vanderbilt Television News Archive</t>
+  </si>
+  <si>
+    <t>Visual Resource Center</t>
   </si>
 </sst>
 </file>
@@ -514,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2902D2F-445E-47D9-918B-A51B6DC5AA7C}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -724,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE82D84-477F-463E-982C-2A37C6B38509}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="E2">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -891,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -916,13 +965,151 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58895BCD-F250-435D-BBCA-E8B9089C4658}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="35.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>